<commit_message>
feat: complete overhaul of Excel pipeline to tracking raw quantities and real-time yfinance valuation computation
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Daily" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Holdings" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,8 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -48,10 +50,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -463,7 +464,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="1" t="n">
         <v>45894</v>
       </c>
       <c r="B2" t="n">
@@ -488,7 +489,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="1" t="n">
         <v>45895</v>
       </c>
       <c r="B3" t="n">
@@ -513,7 +514,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="1" t="n">
         <v>45896</v>
       </c>
       <c r="B4" t="n">
@@ -538,7 +539,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="1" t="n">
         <v>45897</v>
       </c>
       <c r="B5" t="n">
@@ -563,7 +564,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="1" t="n">
         <v>45898</v>
       </c>
       <c r="B6" t="n">
@@ -588,7 +589,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="1" t="n">
         <v>45899</v>
       </c>
       <c r="B7" t="n">
@@ -613,7 +614,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="1" t="n">
         <v>45900</v>
       </c>
       <c r="B8" t="n">
@@ -638,7 +639,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="1" t="n">
         <v>45901</v>
       </c>
       <c r="B9" t="n">
@@ -663,7 +664,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="1" t="n">
         <v>45902</v>
       </c>
       <c r="B10" t="n">
@@ -688,7 +689,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="1" t="n">
         <v>45903</v>
       </c>
       <c r="B11" t="n">
@@ -713,7 +714,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="1" t="n">
         <v>45904</v>
       </c>
       <c r="B12" t="n">
@@ -738,7 +739,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="1" t="n">
         <v>45905</v>
       </c>
       <c r="B13" t="n">
@@ -763,7 +764,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="1" t="n">
         <v>45906</v>
       </c>
       <c r="B14" t="n">
@@ -788,7 +789,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="1" t="n">
         <v>45907</v>
       </c>
       <c r="B15" t="n">
@@ -813,7 +814,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="1" t="n">
         <v>45908</v>
       </c>
       <c r="B16" t="n">
@@ -838,7 +839,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="1" t="n">
         <v>45909</v>
       </c>
       <c r="B17" t="n">
@@ -863,7 +864,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="1" t="n">
         <v>45910</v>
       </c>
       <c r="B18" t="n">
@@ -888,7 +889,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="1" t="n">
         <v>45911</v>
       </c>
       <c r="B19" t="n">
@@ -913,7 +914,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="1" t="n">
         <v>45912</v>
       </c>
       <c r="B20" t="n">
@@ -938,7 +939,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="n">
+      <c r="A21" s="1" t="n">
         <v>45913</v>
       </c>
       <c r="B21" t="n">
@@ -963,7 +964,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="n">
+      <c r="A22" s="1" t="n">
         <v>45914</v>
       </c>
       <c r="B22" t="n">
@@ -988,7 +989,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="n">
+      <c r="A23" s="1" t="n">
         <v>45915</v>
       </c>
       <c r="B23" t="n">
@@ -1013,7 +1014,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="n">
+      <c r="A24" s="1" t="n">
         <v>45916</v>
       </c>
       <c r="B24" t="n">
@@ -1038,7 +1039,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="n">
+      <c r="A25" s="1" t="n">
         <v>45917</v>
       </c>
       <c r="B25" t="n">
@@ -1063,7 +1064,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="1" t="n">
         <v>45918</v>
       </c>
       <c r="B26" t="n">
@@ -1088,7 +1089,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="1" t="n">
         <v>45919</v>
       </c>
       <c r="B27" t="n">
@@ -1113,7 +1114,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="1" t="n">
         <v>45920</v>
       </c>
       <c r="B28" t="n">
@@ -1138,7 +1139,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="1" t="n">
         <v>45921</v>
       </c>
       <c r="B29" t="n">
@@ -1163,7 +1164,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="1" t="n">
         <v>45922</v>
       </c>
       <c r="B30" t="n">
@@ -1188,7 +1189,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="1" t="n">
         <v>45923</v>
       </c>
       <c r="B31" t="n">
@@ -1213,7 +1214,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="n">
+      <c r="A32" s="1" t="n">
         <v>45924</v>
       </c>
       <c r="B32" t="n">
@@ -1238,7 +1239,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="n">
+      <c r="A33" s="1" t="n">
         <v>45925</v>
       </c>
       <c r="B33" t="n">
@@ -1263,7 +1264,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="n">
+      <c r="A34" s="1" t="n">
         <v>45926</v>
       </c>
       <c r="B34" t="n">
@@ -1288,7 +1289,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="n">
+      <c r="A35" s="1" t="n">
         <v>45927</v>
       </c>
       <c r="B35" t="n">
@@ -1313,7 +1314,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="n">
+      <c r="A36" s="1" t="n">
         <v>45928</v>
       </c>
       <c r="B36" t="n">
@@ -1338,7 +1339,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="n">
+      <c r="A37" s="1" t="n">
         <v>45929</v>
       </c>
       <c r="B37" t="n">
@@ -1363,7 +1364,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="n">
+      <c r="A38" s="1" t="n">
         <v>45930</v>
       </c>
       <c r="B38" t="n">
@@ -1388,7 +1389,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="n">
+      <c r="A39" s="1" t="n">
         <v>45931</v>
       </c>
       <c r="B39" t="n">
@@ -1413,7 +1414,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="n">
+      <c r="A40" s="1" t="n">
         <v>45932</v>
       </c>
       <c r="B40" t="n">
@@ -1438,7 +1439,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="n">
+      <c r="A41" s="1" t="n">
         <v>45933</v>
       </c>
       <c r="B41" t="n">
@@ -1463,7 +1464,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="n">
+      <c r="A42" s="1" t="n">
         <v>45934</v>
       </c>
       <c r="B42" t="n">
@@ -1488,7 +1489,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="n">
+      <c r="A43" s="1" t="n">
         <v>45935</v>
       </c>
       <c r="B43" t="n">
@@ -1513,7 +1514,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="n">
+      <c r="A44" s="1" t="n">
         <v>45936</v>
       </c>
       <c r="B44" t="n">
@@ -1538,7 +1539,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="n">
+      <c r="A45" s="1" t="n">
         <v>45937</v>
       </c>
       <c r="B45" t="n">
@@ -1563,7 +1564,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="n">
+      <c r="A46" s="1" t="n">
         <v>45938</v>
       </c>
       <c r="B46" t="n">
@@ -1588,7 +1589,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="n">
+      <c r="A47" s="1" t="n">
         <v>45939</v>
       </c>
       <c r="B47" t="n">
@@ -1613,7 +1614,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="n">
+      <c r="A48" s="1" t="n">
         <v>45940</v>
       </c>
       <c r="B48" t="n">
@@ -1638,7 +1639,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="n">
+      <c r="A49" s="1" t="n">
         <v>45941</v>
       </c>
       <c r="B49" t="n">
@@ -1663,7 +1664,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="n">
+      <c r="A50" s="1" t="n">
         <v>45942</v>
       </c>
       <c r="B50" t="n">
@@ -1688,7 +1689,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="n">
+      <c r="A51" s="1" t="n">
         <v>45943</v>
       </c>
       <c r="B51" t="n">
@@ -1713,7 +1714,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="n">
+      <c r="A52" s="1" t="n">
         <v>45944</v>
       </c>
       <c r="B52" t="n">
@@ -1738,7 +1739,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="n">
+      <c r="A53" s="1" t="n">
         <v>45945</v>
       </c>
       <c r="B53" t="n">
@@ -1763,7 +1764,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="n">
+      <c r="A54" s="1" t="n">
         <v>45946</v>
       </c>
       <c r="B54" t="n">
@@ -1788,7 +1789,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="n">
+      <c r="A55" s="1" t="n">
         <v>45947</v>
       </c>
       <c r="B55" t="n">
@@ -1813,7 +1814,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="n">
+      <c r="A56" s="1" t="n">
         <v>45948</v>
       </c>
       <c r="B56" t="n">
@@ -1838,7 +1839,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="n">
+      <c r="A57" s="1" t="n">
         <v>45949</v>
       </c>
       <c r="B57" t="n">
@@ -1863,7 +1864,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="2" t="n">
+      <c r="A58" s="1" t="n">
         <v>45950</v>
       </c>
       <c r="B58" t="n">
@@ -1888,7 +1889,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="2" t="n">
+      <c r="A59" s="1" t="n">
         <v>45951</v>
       </c>
       <c r="B59" t="n">
@@ -1913,7 +1914,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="2" t="n">
+      <c r="A60" s="1" t="n">
         <v>45952</v>
       </c>
       <c r="B60" t="n">
@@ -1938,7 +1939,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="2" t="n">
+      <c r="A61" s="1" t="n">
         <v>45953</v>
       </c>
       <c r="B61" t="n">
@@ -1963,7 +1964,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="2" t="n">
+      <c r="A62" s="1" t="n">
         <v>45954</v>
       </c>
       <c r="B62" t="n">
@@ -1988,7 +1989,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="2" t="n">
+      <c r="A63" s="1" t="n">
         <v>45955</v>
       </c>
       <c r="B63" t="n">
@@ -2013,7 +2014,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="2" t="n">
+      <c r="A64" s="1" t="n">
         <v>45956</v>
       </c>
       <c r="B64" t="n">
@@ -2038,7 +2039,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="2" t="n">
+      <c r="A65" s="1" t="n">
         <v>45957</v>
       </c>
       <c r="B65" t="n">
@@ -2063,7 +2064,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="2" t="n">
+      <c r="A66" s="1" t="n">
         <v>45958</v>
       </c>
       <c r="B66" t="n">
@@ -2088,7 +2089,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="2" t="n">
+      <c r="A67" s="1" t="n">
         <v>45959</v>
       </c>
       <c r="B67" t="n">
@@ -2113,7 +2114,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="2" t="n">
+      <c r="A68" s="1" t="n">
         <v>45960</v>
       </c>
       <c r="B68" t="n">
@@ -2138,7 +2139,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="n">
+      <c r="A69" s="1" t="n">
         <v>45961</v>
       </c>
       <c r="B69" t="n">
@@ -2163,7 +2164,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="2" t="n">
+      <c r="A70" s="1" t="n">
         <v>45962</v>
       </c>
       <c r="B70" t="n">
@@ -2188,7 +2189,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="2" t="n">
+      <c r="A71" s="1" t="n">
         <v>45963</v>
       </c>
       <c r="B71" t="n">
@@ -2213,7 +2214,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="n">
+      <c r="A72" s="1" t="n">
         <v>45964</v>
       </c>
       <c r="B72" t="n">
@@ -2238,7 +2239,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="2" t="n">
+      <c r="A73" s="1" t="n">
         <v>45965</v>
       </c>
       <c r="B73" t="n">
@@ -2263,7 +2264,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="n">
+      <c r="A74" s="1" t="n">
         <v>45966</v>
       </c>
       <c r="B74" t="n">
@@ -2288,7 +2289,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="2" t="n">
+      <c r="A75" s="1" t="n">
         <v>45967</v>
       </c>
       <c r="B75" t="n">
@@ -2313,7 +2314,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="2" t="n">
+      <c r="A76" s="1" t="n">
         <v>45968</v>
       </c>
       <c r="B76" t="n">
@@ -2338,7 +2339,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="2" t="n">
+      <c r="A77" s="1" t="n">
         <v>45969</v>
       </c>
       <c r="B77" t="n">
@@ -2363,7 +2364,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="2" t="n">
+      <c r="A78" s="1" t="n">
         <v>45970</v>
       </c>
       <c r="B78" t="n">
@@ -2388,7 +2389,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="2" t="n">
+      <c r="A79" s="1" t="n">
         <v>45971</v>
       </c>
       <c r="B79" t="n">
@@ -2413,7 +2414,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="2" t="n">
+      <c r="A80" s="1" t="n">
         <v>45972</v>
       </c>
       <c r="B80" t="n">
@@ -2438,7 +2439,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="2" t="n">
+      <c r="A81" s="1" t="n">
         <v>45973</v>
       </c>
       <c r="B81" t="n">
@@ -2463,7 +2464,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="2" t="n">
+      <c r="A82" s="1" t="n">
         <v>45974</v>
       </c>
       <c r="B82" t="n">
@@ -2488,7 +2489,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="2" t="n">
+      <c r="A83" s="1" t="n">
         <v>45975</v>
       </c>
       <c r="B83" t="n">
@@ -2513,7 +2514,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="n">
+      <c r="A84" s="1" t="n">
         <v>45976</v>
       </c>
       <c r="B84" t="n">
@@ -2538,7 +2539,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="2" t="n">
+      <c r="A85" s="1" t="n">
         <v>45977</v>
       </c>
       <c r="B85" t="n">
@@ -2563,7 +2564,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="n">
+      <c r="A86" s="1" t="n">
         <v>45978</v>
       </c>
       <c r="B86" t="n">
@@ -2588,7 +2589,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="n">
+      <c r="A87" s="1" t="n">
         <v>45979</v>
       </c>
       <c r="B87" t="n">
@@ -2613,7 +2614,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="2" t="n">
+      <c r="A88" s="1" t="n">
         <v>45980</v>
       </c>
       <c r="B88" t="n">
@@ -2638,7 +2639,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="2" t="n">
+      <c r="A89" s="1" t="n">
         <v>45981</v>
       </c>
       <c r="B89" t="n">
@@ -2663,7 +2664,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="2" t="n">
+      <c r="A90" s="1" t="n">
         <v>45982</v>
       </c>
       <c r="B90" t="n">
@@ -2688,7 +2689,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="2" t="n">
+      <c r="A91" s="1" t="n">
         <v>45983</v>
       </c>
       <c r="B91" t="n">
@@ -2713,7 +2714,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="2" t="n">
+      <c r="A92" s="1" t="n">
         <v>45984</v>
       </c>
       <c r="B92" t="n">
@@ -2738,7 +2739,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="n">
+      <c r="A93" s="1" t="n">
         <v>45985</v>
       </c>
       <c r="B93" t="n">
@@ -2763,7 +2764,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="2" t="n">
+      <c r="A94" s="1" t="n">
         <v>45986</v>
       </c>
       <c r="B94" t="n">
@@ -2788,7 +2789,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="2" t="n">
+      <c r="A95" s="1" t="n">
         <v>45987</v>
       </c>
       <c r="B95" t="n">
@@ -2813,7 +2814,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="2" t="n">
+      <c r="A96" s="1" t="n">
         <v>45988</v>
       </c>
       <c r="B96" t="n">
@@ -2838,7 +2839,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="2" t="n">
+      <c r="A97" s="1" t="n">
         <v>45989</v>
       </c>
       <c r="B97" t="n">
@@ -2863,7 +2864,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="2" t="n">
+      <c r="A98" s="1" t="n">
         <v>45990</v>
       </c>
       <c r="B98" t="n">
@@ -2888,7 +2889,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="2" t="n">
+      <c r="A99" s="1" t="n">
         <v>45991</v>
       </c>
       <c r="B99" t="n">
@@ -2913,7 +2914,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="2" t="n">
+      <c r="A100" s="1" t="n">
         <v>45992</v>
       </c>
       <c r="B100" t="n">
@@ -2938,7 +2939,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="2" t="n">
+      <c r="A101" s="1" t="n">
         <v>45993</v>
       </c>
       <c r="B101" t="n">
@@ -2963,7 +2964,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="2" t="n">
+      <c r="A102" s="1" t="n">
         <v>45994</v>
       </c>
       <c r="B102" t="n">
@@ -2988,7 +2989,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="2" t="n">
+      <c r="A103" s="1" t="n">
         <v>45995</v>
       </c>
       <c r="B103" t="n">
@@ -3013,7 +3014,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="2" t="n">
+      <c r="A104" s="1" t="n">
         <v>45996</v>
       </c>
       <c r="B104" t="n">
@@ -3038,7 +3039,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="2" t="n">
+      <c r="A105" s="1" t="n">
         <v>45997</v>
       </c>
       <c r="B105" t="n">
@@ -3063,7 +3064,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="2" t="n">
+      <c r="A106" s="1" t="n">
         <v>45998</v>
       </c>
       <c r="B106" t="n">
@@ -3088,7 +3089,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="2" t="n">
+      <c r="A107" s="1" t="n">
         <v>45999</v>
       </c>
       <c r="B107" t="n">
@@ -3113,7 +3114,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="2" t="n">
+      <c r="A108" s="1" t="n">
         <v>46000</v>
       </c>
       <c r="B108" t="n">
@@ -3138,7 +3139,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="2" t="n">
+      <c r="A109" s="1" t="n">
         <v>46001</v>
       </c>
       <c r="B109" t="n">
@@ -3163,7 +3164,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="2" t="n">
+      <c r="A110" s="1" t="n">
         <v>46002</v>
       </c>
       <c r="B110" t="n">
@@ -3188,7 +3189,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="2" t="n">
+      <c r="A111" s="1" t="n">
         <v>46003</v>
       </c>
       <c r="B111" t="n">
@@ -3213,7 +3214,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="2" t="n">
+      <c r="A112" s="1" t="n">
         <v>46004</v>
       </c>
       <c r="B112" t="n">
@@ -3238,7 +3239,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="2" t="n">
+      <c r="A113" s="1" t="n">
         <v>46005</v>
       </c>
       <c r="B113" t="n">
@@ -3263,7 +3264,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="2" t="n">
+      <c r="A114" s="1" t="n">
         <v>46006</v>
       </c>
       <c r="B114" t="n">
@@ -3288,7 +3289,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="2" t="n">
+      <c r="A115" s="1" t="n">
         <v>46007</v>
       </c>
       <c r="B115" t="n">
@@ -3313,7 +3314,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="2" t="n">
+      <c r="A116" s="1" t="n">
         <v>46008</v>
       </c>
       <c r="B116" t="n">
@@ -3338,7 +3339,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="2" t="n">
+      <c r="A117" s="1" t="n">
         <v>46009</v>
       </c>
       <c r="B117" t="n">
@@ -3363,7 +3364,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="2" t="n">
+      <c r="A118" s="1" t="n">
         <v>46010</v>
       </c>
       <c r="B118" t="n">
@@ -3388,7 +3389,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="2" t="n">
+      <c r="A119" s="1" t="n">
         <v>46011</v>
       </c>
       <c r="B119" t="n">
@@ -3413,7 +3414,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="2" t="n">
+      <c r="A120" s="1" t="n">
         <v>46012</v>
       </c>
       <c r="B120" t="n">
@@ -3438,7 +3439,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="2" t="n">
+      <c r="A121" s="1" t="n">
         <v>46013</v>
       </c>
       <c r="B121" t="n">
@@ -3463,7 +3464,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="2" t="n">
+      <c r="A122" s="1" t="n">
         <v>46014</v>
       </c>
       <c r="B122" t="n">
@@ -3488,7 +3489,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="2" t="n">
+      <c r="A123" s="1" t="n">
         <v>46015</v>
       </c>
       <c r="B123" t="n">
@@ -3513,7 +3514,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="2" t="n">
+      <c r="A124" s="1" t="n">
         <v>46016</v>
       </c>
       <c r="B124" t="n">
@@ -3538,7 +3539,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="2" t="n">
+      <c r="A125" s="1" t="n">
         <v>46017</v>
       </c>
       <c r="B125" t="n">
@@ -3563,7 +3564,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="2" t="n">
+      <c r="A126" s="1" t="n">
         <v>46018</v>
       </c>
       <c r="B126" t="n">
@@ -3588,7 +3589,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="2" t="n">
+      <c r="A127" s="1" t="n">
         <v>46019</v>
       </c>
       <c r="B127" t="n">
@@ -3613,7 +3614,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="2" t="n">
+      <c r="A128" s="1" t="n">
         <v>46020</v>
       </c>
       <c r="B128" t="n">
@@ -3638,7 +3639,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="2" t="n">
+      <c r="A129" s="1" t="n">
         <v>46021</v>
       </c>
       <c r="B129" t="n">
@@ -3663,7 +3664,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="2" t="n">
+      <c r="A130" s="1" t="n">
         <v>46022</v>
       </c>
       <c r="B130" t="n">
@@ -3688,7 +3689,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="2" t="n">
+      <c r="A131" s="1" t="n">
         <v>46023</v>
       </c>
       <c r="B131" t="n">
@@ -3713,7 +3714,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="2" t="n">
+      <c r="A132" s="1" t="n">
         <v>46024</v>
       </c>
       <c r="B132" t="n">
@@ -3738,7 +3739,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="2" t="n">
+      <c r="A133" s="1" t="n">
         <v>46025</v>
       </c>
       <c r="B133" t="n">
@@ -3763,7 +3764,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="2" t="n">
+      <c r="A134" s="1" t="n">
         <v>46026</v>
       </c>
       <c r="B134" t="n">
@@ -3788,7 +3789,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="2" t="n">
+      <c r="A135" s="1" t="n">
         <v>46027</v>
       </c>
       <c r="B135" t="n">
@@ -3813,7 +3814,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="2" t="n">
+      <c r="A136" s="1" t="n">
         <v>46028</v>
       </c>
       <c r="B136" t="n">
@@ -3838,7 +3839,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="2" t="n">
+      <c r="A137" s="1" t="n">
         <v>46029</v>
       </c>
       <c r="B137" t="n">
@@ -3863,7 +3864,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="2" t="n">
+      <c r="A138" s="1" t="n">
         <v>46030</v>
       </c>
       <c r="B138" t="n">
@@ -3888,7 +3889,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="2" t="n">
+      <c r="A139" s="1" t="n">
         <v>46031</v>
       </c>
       <c r="B139" t="n">
@@ -3913,7 +3914,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="2" t="n">
+      <c r="A140" s="1" t="n">
         <v>46032</v>
       </c>
       <c r="B140" t="n">
@@ -3938,7 +3939,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="2" t="n">
+      <c r="A141" s="1" t="n">
         <v>46033</v>
       </c>
       <c r="B141" t="n">
@@ -3963,7 +3964,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="2" t="n">
+      <c r="A142" s="1" t="n">
         <v>46034</v>
       </c>
       <c r="B142" t="n">
@@ -3988,7 +3989,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="2" t="n">
+      <c r="A143" s="1" t="n">
         <v>46035</v>
       </c>
       <c r="B143" t="n">
@@ -4013,7 +4014,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="2" t="n">
+      <c r="A144" s="1" t="n">
         <v>46036</v>
       </c>
       <c r="B144" t="n">
@@ -4038,7 +4039,7 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="2" t="n">
+      <c r="A145" s="1" t="n">
         <v>46037</v>
       </c>
       <c r="B145" t="n">
@@ -4063,7 +4064,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="2" t="n">
+      <c r="A146" s="1" t="n">
         <v>46038</v>
       </c>
       <c r="B146" t="n">
@@ -4088,7 +4089,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="2" t="n">
+      <c r="A147" s="1" t="n">
         <v>46039</v>
       </c>
       <c r="B147" t="n">
@@ -4113,7 +4114,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="2" t="n">
+      <c r="A148" s="1" t="n">
         <v>46040</v>
       </c>
       <c r="B148" t="n">
@@ -4138,7 +4139,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="2" t="n">
+      <c r="A149" s="1" t="n">
         <v>46041</v>
       </c>
       <c r="B149" t="n">
@@ -4163,7 +4164,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="2" t="n">
+      <c r="A150" s="1" t="n">
         <v>46042</v>
       </c>
       <c r="B150" t="n">
@@ -4188,7 +4189,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="2" t="n">
+      <c r="A151" s="1" t="n">
         <v>46043</v>
       </c>
       <c r="B151" t="n">
@@ -4213,7 +4214,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="2" t="n">
+      <c r="A152" s="1" t="n">
         <v>46044</v>
       </c>
       <c r="B152" t="n">
@@ -4238,7 +4239,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="2" t="n">
+      <c r="A153" s="1" t="n">
         <v>46045</v>
       </c>
       <c r="B153" t="n">
@@ -4263,7 +4264,7 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="2" t="n">
+      <c r="A154" s="1" t="n">
         <v>46046</v>
       </c>
       <c r="B154" t="n">
@@ -4288,7 +4289,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="2" t="n">
+      <c r="A155" s="1" t="n">
         <v>46047</v>
       </c>
       <c r="B155" t="n">
@@ -4313,7 +4314,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="2" t="n">
+      <c r="A156" s="1" t="n">
         <v>46048</v>
       </c>
       <c r="B156" t="n">
@@ -4338,7 +4339,7 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="2" t="n">
+      <c r="A157" s="1" t="n">
         <v>46049</v>
       </c>
       <c r="B157" t="n">
@@ -4363,7 +4364,7 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="2" t="n">
+      <c r="A158" s="1" t="n">
         <v>46050</v>
       </c>
       <c r="B158" t="n">
@@ -4388,7 +4389,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="2" t="n">
+      <c r="A159" s="1" t="n">
         <v>46051</v>
       </c>
       <c r="B159" t="n">
@@ -4413,7 +4414,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="2" t="n">
+      <c r="A160" s="1" t="n">
         <v>46052</v>
       </c>
       <c r="B160" t="n">
@@ -4438,7 +4439,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="2" t="n">
+      <c r="A161" s="1" t="n">
         <v>46053</v>
       </c>
       <c r="B161" t="n">
@@ -4463,7 +4464,7 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="2" t="n">
+      <c r="A162" s="1" t="n">
         <v>46054</v>
       </c>
       <c r="B162" t="n">
@@ -4488,7 +4489,7 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="2" t="n">
+      <c r="A163" s="1" t="n">
         <v>46055</v>
       </c>
       <c r="B163" t="n">
@@ -4513,7 +4514,7 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="2" t="n">
+      <c r="A164" s="1" t="n">
         <v>46056</v>
       </c>
       <c r="B164" t="n">
@@ -4538,7 +4539,7 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="2" t="n">
+      <c r="A165" s="1" t="n">
         <v>46057</v>
       </c>
       <c r="B165" t="n">
@@ -4563,7 +4564,7 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="2" t="n">
+      <c r="A166" s="1" t="n">
         <v>46058</v>
       </c>
       <c r="B166" t="n">
@@ -4588,7 +4589,7 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="2" t="n">
+      <c r="A167" s="1" t="n">
         <v>46059</v>
       </c>
       <c r="B167" t="n">
@@ -4613,7 +4614,7 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="2" t="n">
+      <c r="A168" s="1" t="n">
         <v>46060</v>
       </c>
       <c r="B168" t="n">
@@ -4638,7 +4639,7 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="2" t="n">
+      <c r="A169" s="1" t="n">
         <v>46061</v>
       </c>
       <c r="B169" t="n">
@@ -4663,7 +4664,7 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="2" t="n">
+      <c r="A170" s="1" t="n">
         <v>46062</v>
       </c>
       <c r="B170" t="n">
@@ -4688,7 +4689,7 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="2" t="n">
+      <c r="A171" s="1" t="n">
         <v>46063</v>
       </c>
       <c r="B171" t="n">
@@ -4713,7 +4714,7 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="2" t="n">
+      <c r="A172" s="1" t="n">
         <v>46064</v>
       </c>
       <c r="B172" t="n">
@@ -4738,7 +4739,7 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="2" t="n">
+      <c r="A173" s="1" t="n">
         <v>46065</v>
       </c>
       <c r="B173" t="n">
@@ -4763,7 +4764,7 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="2" t="n">
+      <c r="A174" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="B174" t="n">
@@ -4788,7 +4789,7 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="2" t="n">
+      <c r="A175" s="1" t="n">
         <v>46067</v>
       </c>
       <c r="B175" t="n">
@@ -4813,7 +4814,7 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="2" t="n">
+      <c r="A176" s="1" t="n">
         <v>46068</v>
       </c>
       <c r="B176" t="n">
@@ -4838,7 +4839,7 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="2" t="n">
+      <c r="A177" s="1" t="n">
         <v>46069</v>
       </c>
       <c r="B177" t="n">
@@ -4863,7 +4864,7 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="2" t="n">
+      <c r="A178" s="1" t="n">
         <v>46070</v>
       </c>
       <c r="B178" t="n">
@@ -4888,7 +4889,7 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="2" t="n">
+      <c r="A179" s="1" t="n">
         <v>46071</v>
       </c>
       <c r="B179" t="n">
@@ -4913,7 +4914,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="2" t="n">
+      <c r="A180" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="B180" t="n">
@@ -4938,7 +4939,7 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" s="2" t="n">
+      <c r="A181" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="B181" t="n">
@@ -4963,7 +4964,7 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="2" t="n">
+      <c r="A182" s="1" t="n">
         <v>46074</v>
       </c>
       <c r="B182" t="n">
@@ -4988,7 +4989,7 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" s="2" t="n">
+      <c r="A183" s="1" t="n">
         <v>46075</v>
       </c>
       <c r="B183" t="n">
@@ -5013,7 +5014,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="2" t="n">
+      <c r="A184" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="B184" t="n">
@@ -5033,6 +5034,102 @@
       </c>
       <c r="G184" t="n">
         <v>2989.41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CASH</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>USD Cash</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>571.73</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>GC=F</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Gold Futures</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.287</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>NVIDIA Corp</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>17.4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Tesla Inc</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(excel): restore native formatting and elegantly inject Holdings sheet using openpyxl
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -17,17 +17,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -50,9 +52,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -464,7 +468,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>45894</v>
       </c>
       <c r="B2" t="n">
@@ -489,7 +493,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>45895</v>
       </c>
       <c r="B3" t="n">
@@ -514,7 +518,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>45896</v>
       </c>
       <c r="B4" t="n">
@@ -539,7 +543,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>45897</v>
       </c>
       <c r="B5" t="n">
@@ -564,7 +568,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>45898</v>
       </c>
       <c r="B6" t="n">
@@ -589,7 +593,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <v>45899</v>
       </c>
       <c r="B7" t="n">
@@ -614,7 +618,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>45900</v>
       </c>
       <c r="B8" t="n">
@@ -639,7 +643,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <v>45901</v>
       </c>
       <c r="B9" t="n">
@@ -664,7 +668,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="2" t="n">
         <v>45902</v>
       </c>
       <c r="B10" t="n">
@@ -689,7 +693,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="2" t="n">
         <v>45903</v>
       </c>
       <c r="B11" t="n">
@@ -714,7 +718,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="2" t="n">
         <v>45904</v>
       </c>
       <c r="B12" t="n">
@@ -739,7 +743,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="2" t="n">
         <v>45905</v>
       </c>
       <c r="B13" t="n">
@@ -764,7 +768,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="2" t="n">
         <v>45906</v>
       </c>
       <c r="B14" t="n">
@@ -789,7 +793,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="2" t="n">
         <v>45907</v>
       </c>
       <c r="B15" t="n">
@@ -814,7 +818,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="2" t="n">
         <v>45908</v>
       </c>
       <c r="B16" t="n">
@@ -839,7 +843,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="2" t="n">
         <v>45909</v>
       </c>
       <c r="B17" t="n">
@@ -864,7 +868,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="2" t="n">
         <v>45910</v>
       </c>
       <c r="B18" t="n">
@@ -889,7 +893,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="2" t="n">
         <v>45911</v>
       </c>
       <c r="B19" t="n">
@@ -914,7 +918,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="2" t="n">
         <v>45912</v>
       </c>
       <c r="B20" t="n">
@@ -939,7 +943,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="2" t="n">
         <v>45913</v>
       </c>
       <c r="B21" t="n">
@@ -964,7 +968,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="2" t="n">
         <v>45914</v>
       </c>
       <c r="B22" t="n">
@@ -989,7 +993,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="2" t="n">
         <v>45915</v>
       </c>
       <c r="B23" t="n">
@@ -1014,7 +1018,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="2" t="n">
         <v>45916</v>
       </c>
       <c r="B24" t="n">
@@ -1039,7 +1043,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="2" t="n">
         <v>45917</v>
       </c>
       <c r="B25" t="n">
@@ -1064,7 +1068,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="2" t="n">
         <v>45918</v>
       </c>
       <c r="B26" t="n">
@@ -1089,7 +1093,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
+      <c r="A27" s="2" t="n">
         <v>45919</v>
       </c>
       <c r="B27" t="n">
@@ -1114,7 +1118,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
+      <c r="A28" s="2" t="n">
         <v>45920</v>
       </c>
       <c r="B28" t="n">
@@ -1139,7 +1143,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="2" t="n">
         <v>45921</v>
       </c>
       <c r="B29" t="n">
@@ -1164,7 +1168,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
+      <c r="A30" s="2" t="n">
         <v>45922</v>
       </c>
       <c r="B30" t="n">
@@ -1189,7 +1193,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
+      <c r="A31" s="2" t="n">
         <v>45923</v>
       </c>
       <c r="B31" t="n">
@@ -1214,7 +1218,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
+      <c r="A32" s="2" t="n">
         <v>45924</v>
       </c>
       <c r="B32" t="n">
@@ -1239,7 +1243,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="2" t="n">
         <v>45925</v>
       </c>
       <c r="B33" t="n">
@@ -1264,7 +1268,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n">
+      <c r="A34" s="2" t="n">
         <v>45926</v>
       </c>
       <c r="B34" t="n">
@@ -1289,7 +1293,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n">
+      <c r="A35" s="2" t="n">
         <v>45927</v>
       </c>
       <c r="B35" t="n">
@@ -1314,7 +1318,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
+      <c r="A36" s="2" t="n">
         <v>45928</v>
       </c>
       <c r="B36" t="n">
@@ -1339,7 +1343,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n">
+      <c r="A37" s="2" t="n">
         <v>45929</v>
       </c>
       <c r="B37" t="n">
@@ -1364,7 +1368,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n">
+      <c r="A38" s="2" t="n">
         <v>45930</v>
       </c>
       <c r="B38" t="n">
@@ -1389,7 +1393,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n">
+      <c r="A39" s="2" t="n">
         <v>45931</v>
       </c>
       <c r="B39" t="n">
@@ -1414,7 +1418,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n">
+      <c r="A40" s="2" t="n">
         <v>45932</v>
       </c>
       <c r="B40" t="n">
@@ -1439,7 +1443,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="2" t="n">
         <v>45933</v>
       </c>
       <c r="B41" t="n">
@@ -1464,7 +1468,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n">
+      <c r="A42" s="2" t="n">
         <v>45934</v>
       </c>
       <c r="B42" t="n">
@@ -1489,7 +1493,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n">
+      <c r="A43" s="2" t="n">
         <v>45935</v>
       </c>
       <c r="B43" t="n">
@@ -1514,7 +1518,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n">
+      <c r="A44" s="2" t="n">
         <v>45936</v>
       </c>
       <c r="B44" t="n">
@@ -1539,7 +1543,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="n">
+      <c r="A45" s="2" t="n">
         <v>45937</v>
       </c>
       <c r="B45" t="n">
@@ -1564,7 +1568,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n">
+      <c r="A46" s="2" t="n">
         <v>45938</v>
       </c>
       <c r="B46" t="n">
@@ -1589,7 +1593,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n">
+      <c r="A47" s="2" t="n">
         <v>45939</v>
       </c>
       <c r="B47" t="n">
@@ -1614,7 +1618,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n">
+      <c r="A48" s="2" t="n">
         <v>45940</v>
       </c>
       <c r="B48" t="n">
@@ -1639,7 +1643,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n">
+      <c r="A49" s="2" t="n">
         <v>45941</v>
       </c>
       <c r="B49" t="n">
@@ -1664,7 +1668,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n">
+      <c r="A50" s="2" t="n">
         <v>45942</v>
       </c>
       <c r="B50" t="n">
@@ -1689,7 +1693,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="n">
+      <c r="A51" s="2" t="n">
         <v>45943</v>
       </c>
       <c r="B51" t="n">
@@ -1714,7 +1718,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="n">
+      <c r="A52" s="2" t="n">
         <v>45944</v>
       </c>
       <c r="B52" t="n">
@@ -1739,7 +1743,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n">
+      <c r="A53" s="2" t="n">
         <v>45945</v>
       </c>
       <c r="B53" t="n">
@@ -1764,7 +1768,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="n">
+      <c r="A54" s="2" t="n">
         <v>45946</v>
       </c>
       <c r="B54" t="n">
@@ -1789,7 +1793,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="n">
+      <c r="A55" s="2" t="n">
         <v>45947</v>
       </c>
       <c r="B55" t="n">
@@ -1814,7 +1818,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="2" t="n">
         <v>45948</v>
       </c>
       <c r="B56" t="n">
@@ -1839,7 +1843,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="n">
+      <c r="A57" s="2" t="n">
         <v>45949</v>
       </c>
       <c r="B57" t="n">
@@ -1864,7 +1868,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="n">
+      <c r="A58" s="2" t="n">
         <v>45950</v>
       </c>
       <c r="B58" t="n">
@@ -1889,7 +1893,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="2" t="n">
         <v>45951</v>
       </c>
       <c r="B59" t="n">
@@ -1914,7 +1918,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="2" t="n">
         <v>45952</v>
       </c>
       <c r="B60" t="n">
@@ -1939,7 +1943,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="2" t="n">
         <v>45953</v>
       </c>
       <c r="B61" t="n">
@@ -1964,7 +1968,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="2" t="n">
         <v>45954</v>
       </c>
       <c r="B62" t="n">
@@ -1989,7 +1993,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="2" t="n">
         <v>45955</v>
       </c>
       <c r="B63" t="n">
@@ -2014,7 +2018,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="2" t="n">
         <v>45956</v>
       </c>
       <c r="B64" t="n">
@@ -2039,7 +2043,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="n">
+      <c r="A65" s="2" t="n">
         <v>45957</v>
       </c>
       <c r="B65" t="n">
@@ -2064,7 +2068,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="2" t="n">
         <v>45958</v>
       </c>
       <c r="B66" t="n">
@@ -2089,7 +2093,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="n">
+      <c r="A67" s="2" t="n">
         <v>45959</v>
       </c>
       <c r="B67" t="n">
@@ -2114,7 +2118,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="n">
+      <c r="A68" s="2" t="n">
         <v>45960</v>
       </c>
       <c r="B68" t="n">
@@ -2139,7 +2143,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="n">
+      <c r="A69" s="2" t="n">
         <v>45961</v>
       </c>
       <c r="B69" t="n">
@@ -2164,7 +2168,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="n">
+      <c r="A70" s="2" t="n">
         <v>45962</v>
       </c>
       <c r="B70" t="n">
@@ -2189,7 +2193,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="n">
+      <c r="A71" s="2" t="n">
         <v>45963</v>
       </c>
       <c r="B71" t="n">
@@ -2214,7 +2218,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="n">
+      <c r="A72" s="2" t="n">
         <v>45964</v>
       </c>
       <c r="B72" t="n">
@@ -2239,7 +2243,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="n">
+      <c r="A73" s="2" t="n">
         <v>45965</v>
       </c>
       <c r="B73" t="n">
@@ -2264,7 +2268,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="n">
+      <c r="A74" s="2" t="n">
         <v>45966</v>
       </c>
       <c r="B74" t="n">
@@ -2289,7 +2293,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="n">
+      <c r="A75" s="2" t="n">
         <v>45967</v>
       </c>
       <c r="B75" t="n">
@@ -2314,7 +2318,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="n">
+      <c r="A76" s="2" t="n">
         <v>45968</v>
       </c>
       <c r="B76" t="n">
@@ -2339,7 +2343,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="n">
+      <c r="A77" s="2" t="n">
         <v>45969</v>
       </c>
       <c r="B77" t="n">
@@ -2364,7 +2368,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="n">
+      <c r="A78" s="2" t="n">
         <v>45970</v>
       </c>
       <c r="B78" t="n">
@@ -2389,7 +2393,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="n">
+      <c r="A79" s="2" t="n">
         <v>45971</v>
       </c>
       <c r="B79" t="n">
@@ -2414,7 +2418,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="n">
+      <c r="A80" s="2" t="n">
         <v>45972</v>
       </c>
       <c r="B80" t="n">
@@ -2439,7 +2443,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="n">
+      <c r="A81" s="2" t="n">
         <v>45973</v>
       </c>
       <c r="B81" t="n">
@@ -2464,7 +2468,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="n">
+      <c r="A82" s="2" t="n">
         <v>45974</v>
       </c>
       <c r="B82" t="n">
@@ -2489,7 +2493,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="n">
+      <c r="A83" s="2" t="n">
         <v>45975</v>
       </c>
       <c r="B83" t="n">
@@ -2514,7 +2518,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="n">
+      <c r="A84" s="2" t="n">
         <v>45976</v>
       </c>
       <c r="B84" t="n">
@@ -2539,7 +2543,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="1" t="n">
+      <c r="A85" s="2" t="n">
         <v>45977</v>
       </c>
       <c r="B85" t="n">
@@ -2564,7 +2568,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="n">
+      <c r="A86" s="2" t="n">
         <v>45978</v>
       </c>
       <c r="B86" t="n">
@@ -2589,7 +2593,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1" t="n">
+      <c r="A87" s="2" t="n">
         <v>45979</v>
       </c>
       <c r="B87" t="n">
@@ -2614,7 +2618,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1" t="n">
+      <c r="A88" s="2" t="n">
         <v>45980</v>
       </c>
       <c r="B88" t="n">
@@ -2639,7 +2643,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="1" t="n">
+      <c r="A89" s="2" t="n">
         <v>45981</v>
       </c>
       <c r="B89" t="n">
@@ -2664,7 +2668,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="1" t="n">
+      <c r="A90" s="2" t="n">
         <v>45982</v>
       </c>
       <c r="B90" t="n">
@@ -2689,7 +2693,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="n">
+      <c r="A91" s="2" t="n">
         <v>45983</v>
       </c>
       <c r="B91" t="n">
@@ -2714,7 +2718,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="n">
+      <c r="A92" s="2" t="n">
         <v>45984</v>
       </c>
       <c r="B92" t="n">
@@ -2739,7 +2743,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="n">
+      <c r="A93" s="2" t="n">
         <v>45985</v>
       </c>
       <c r="B93" t="n">
@@ -2764,7 +2768,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="1" t="n">
+      <c r="A94" s="2" t="n">
         <v>45986</v>
       </c>
       <c r="B94" t="n">
@@ -2789,7 +2793,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="1" t="n">
+      <c r="A95" s="2" t="n">
         <v>45987</v>
       </c>
       <c r="B95" t="n">
@@ -2814,7 +2818,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="1" t="n">
+      <c r="A96" s="2" t="n">
         <v>45988</v>
       </c>
       <c r="B96" t="n">
@@ -2839,7 +2843,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="1" t="n">
+      <c r="A97" s="2" t="n">
         <v>45989</v>
       </c>
       <c r="B97" t="n">
@@ -2864,7 +2868,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="n">
+      <c r="A98" s="2" t="n">
         <v>45990</v>
       </c>
       <c r="B98" t="n">
@@ -2889,7 +2893,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="1" t="n">
+      <c r="A99" s="2" t="n">
         <v>45991</v>
       </c>
       <c r="B99" t="n">
@@ -2914,7 +2918,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="n">
+      <c r="A100" s="2" t="n">
         <v>45992</v>
       </c>
       <c r="B100" t="n">
@@ -2939,7 +2943,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="1" t="n">
+      <c r="A101" s="2" t="n">
         <v>45993</v>
       </c>
       <c r="B101" t="n">
@@ -2964,7 +2968,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="n">
+      <c r="A102" s="2" t="n">
         <v>45994</v>
       </c>
       <c r="B102" t="n">
@@ -2989,7 +2993,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="n">
+      <c r="A103" s="2" t="n">
         <v>45995</v>
       </c>
       <c r="B103" t="n">
@@ -3014,7 +3018,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="1" t="n">
+      <c r="A104" s="2" t="n">
         <v>45996</v>
       </c>
       <c r="B104" t="n">
@@ -3039,7 +3043,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="1" t="n">
+      <c r="A105" s="2" t="n">
         <v>45997</v>
       </c>
       <c r="B105" t="n">
@@ -3064,7 +3068,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="n">
+      <c r="A106" s="2" t="n">
         <v>45998</v>
       </c>
       <c r="B106" t="n">
@@ -3089,7 +3093,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="n">
+      <c r="A107" s="2" t="n">
         <v>45999</v>
       </c>
       <c r="B107" t="n">
@@ -3114,7 +3118,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="n">
+      <c r="A108" s="2" t="n">
         <v>46000</v>
       </c>
       <c r="B108" t="n">
@@ -3139,7 +3143,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="n">
+      <c r="A109" s="2" t="n">
         <v>46001</v>
       </c>
       <c r="B109" t="n">
@@ -3164,7 +3168,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="n">
+      <c r="A110" s="2" t="n">
         <v>46002</v>
       </c>
       <c r="B110" t="n">
@@ -3189,7 +3193,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="n">
+      <c r="A111" s="2" t="n">
         <v>46003</v>
       </c>
       <c r="B111" t="n">
@@ -3214,7 +3218,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="n">
+      <c r="A112" s="2" t="n">
         <v>46004</v>
       </c>
       <c r="B112" t="n">
@@ -3239,7 +3243,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="1" t="n">
+      <c r="A113" s="2" t="n">
         <v>46005</v>
       </c>
       <c r="B113" t="n">
@@ -3264,7 +3268,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="1" t="n">
+      <c r="A114" s="2" t="n">
         <v>46006</v>
       </c>
       <c r="B114" t="n">
@@ -3289,7 +3293,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="n">
+      <c r="A115" s="2" t="n">
         <v>46007</v>
       </c>
       <c r="B115" t="n">
@@ -3314,7 +3318,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="1" t="n">
+      <c r="A116" s="2" t="n">
         <v>46008</v>
       </c>
       <c r="B116" t="n">
@@ -3339,7 +3343,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="1" t="n">
+      <c r="A117" s="2" t="n">
         <v>46009</v>
       </c>
       <c r="B117" t="n">
@@ -3364,7 +3368,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="n">
+      <c r="A118" s="2" t="n">
         <v>46010</v>
       </c>
       <c r="B118" t="n">
@@ -3389,7 +3393,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="1" t="n">
+      <c r="A119" s="2" t="n">
         <v>46011</v>
       </c>
       <c r="B119" t="n">
@@ -3414,7 +3418,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="1" t="n">
+      <c r="A120" s="2" t="n">
         <v>46012</v>
       </c>
       <c r="B120" t="n">
@@ -3439,7 +3443,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="1" t="n">
+      <c r="A121" s="2" t="n">
         <v>46013</v>
       </c>
       <c r="B121" t="n">
@@ -3464,7 +3468,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="n">
+      <c r="A122" s="2" t="n">
         <v>46014</v>
       </c>
       <c r="B122" t="n">
@@ -3489,7 +3493,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="1" t="n">
+      <c r="A123" s="2" t="n">
         <v>46015</v>
       </c>
       <c r="B123" t="n">
@@ -3514,7 +3518,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="1" t="n">
+      <c r="A124" s="2" t="n">
         <v>46016</v>
       </c>
       <c r="B124" t="n">
@@ -3539,7 +3543,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="1" t="n">
+      <c r="A125" s="2" t="n">
         <v>46017</v>
       </c>
       <c r="B125" t="n">
@@ -3564,7 +3568,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="1" t="n">
+      <c r="A126" s="2" t="n">
         <v>46018</v>
       </c>
       <c r="B126" t="n">
@@ -3589,7 +3593,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="1" t="n">
+      <c r="A127" s="2" t="n">
         <v>46019</v>
       </c>
       <c r="B127" t="n">
@@ -3614,7 +3618,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="1" t="n">
+      <c r="A128" s="2" t="n">
         <v>46020</v>
       </c>
       <c r="B128" t="n">
@@ -3639,7 +3643,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="1" t="n">
+      <c r="A129" s="2" t="n">
         <v>46021</v>
       </c>
       <c r="B129" t="n">
@@ -3664,7 +3668,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="1" t="n">
+      <c r="A130" s="2" t="n">
         <v>46022</v>
       </c>
       <c r="B130" t="n">
@@ -3689,7 +3693,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="1" t="n">
+      <c r="A131" s="2" t="n">
         <v>46023</v>
       </c>
       <c r="B131" t="n">
@@ -3714,7 +3718,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="1" t="n">
+      <c r="A132" s="2" t="n">
         <v>46024</v>
       </c>
       <c r="B132" t="n">
@@ -3739,7 +3743,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="1" t="n">
+      <c r="A133" s="2" t="n">
         <v>46025</v>
       </c>
       <c r="B133" t="n">
@@ -3764,7 +3768,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="1" t="n">
+      <c r="A134" s="2" t="n">
         <v>46026</v>
       </c>
       <c r="B134" t="n">
@@ -3789,7 +3793,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="1" t="n">
+      <c r="A135" s="2" t="n">
         <v>46027</v>
       </c>
       <c r="B135" t="n">
@@ -3814,7 +3818,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="1" t="n">
+      <c r="A136" s="2" t="n">
         <v>46028</v>
       </c>
       <c r="B136" t="n">
@@ -3839,7 +3843,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="1" t="n">
+      <c r="A137" s="2" t="n">
         <v>46029</v>
       </c>
       <c r="B137" t="n">
@@ -3864,7 +3868,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="1" t="n">
+      <c r="A138" s="2" t="n">
         <v>46030</v>
       </c>
       <c r="B138" t="n">
@@ -3889,7 +3893,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="1" t="n">
+      <c r="A139" s="2" t="n">
         <v>46031</v>
       </c>
       <c r="B139" t="n">
@@ -3914,7 +3918,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="1" t="n">
+      <c r="A140" s="2" t="n">
         <v>46032</v>
       </c>
       <c r="B140" t="n">
@@ -3939,7 +3943,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="1" t="n">
+      <c r="A141" s="2" t="n">
         <v>46033</v>
       </c>
       <c r="B141" t="n">
@@ -3964,7 +3968,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="1" t="n">
+      <c r="A142" s="2" t="n">
         <v>46034</v>
       </c>
       <c r="B142" t="n">
@@ -3989,7 +3993,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="1" t="n">
+      <c r="A143" s="2" t="n">
         <v>46035</v>
       </c>
       <c r="B143" t="n">
@@ -4014,7 +4018,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="1" t="n">
+      <c r="A144" s="2" t="n">
         <v>46036</v>
       </c>
       <c r="B144" t="n">
@@ -4039,7 +4043,7 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="1" t="n">
+      <c r="A145" s="2" t="n">
         <v>46037</v>
       </c>
       <c r="B145" t="n">
@@ -4064,7 +4068,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="1" t="n">
+      <c r="A146" s="2" t="n">
         <v>46038</v>
       </c>
       <c r="B146" t="n">
@@ -4089,7 +4093,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="1" t="n">
+      <c r="A147" s="2" t="n">
         <v>46039</v>
       </c>
       <c r="B147" t="n">
@@ -4114,7 +4118,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="1" t="n">
+      <c r="A148" s="2" t="n">
         <v>46040</v>
       </c>
       <c r="B148" t="n">
@@ -4139,7 +4143,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="1" t="n">
+      <c r="A149" s="2" t="n">
         <v>46041</v>
       </c>
       <c r="B149" t="n">
@@ -4164,7 +4168,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="1" t="n">
+      <c r="A150" s="2" t="n">
         <v>46042</v>
       </c>
       <c r="B150" t="n">
@@ -4189,7 +4193,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="1" t="n">
+      <c r="A151" s="2" t="n">
         <v>46043</v>
       </c>
       <c r="B151" t="n">
@@ -4214,7 +4218,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="1" t="n">
+      <c r="A152" s="2" t="n">
         <v>46044</v>
       </c>
       <c r="B152" t="n">
@@ -4239,7 +4243,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="1" t="n">
+      <c r="A153" s="2" t="n">
         <v>46045</v>
       </c>
       <c r="B153" t="n">
@@ -4264,7 +4268,7 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="1" t="n">
+      <c r="A154" s="2" t="n">
         <v>46046</v>
       </c>
       <c r="B154" t="n">
@@ -4289,7 +4293,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="1" t="n">
+      <c r="A155" s="2" t="n">
         <v>46047</v>
       </c>
       <c r="B155" t="n">
@@ -4314,7 +4318,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="1" t="n">
+      <c r="A156" s="2" t="n">
         <v>46048</v>
       </c>
       <c r="B156" t="n">
@@ -4339,7 +4343,7 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="1" t="n">
+      <c r="A157" s="2" t="n">
         <v>46049</v>
       </c>
       <c r="B157" t="n">
@@ -4364,7 +4368,7 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="1" t="n">
+      <c r="A158" s="2" t="n">
         <v>46050</v>
       </c>
       <c r="B158" t="n">
@@ -4389,7 +4393,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="1" t="n">
+      <c r="A159" s="2" t="n">
         <v>46051</v>
       </c>
       <c r="B159" t="n">
@@ -4414,7 +4418,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="1" t="n">
+      <c r="A160" s="2" t="n">
         <v>46052</v>
       </c>
       <c r="B160" t="n">
@@ -4439,7 +4443,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="1" t="n">
+      <c r="A161" s="2" t="n">
         <v>46053</v>
       </c>
       <c r="B161" t="n">
@@ -4464,7 +4468,7 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="1" t="n">
+      <c r="A162" s="2" t="n">
         <v>46054</v>
       </c>
       <c r="B162" t="n">
@@ -4489,7 +4493,7 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="1" t="n">
+      <c r="A163" s="2" t="n">
         <v>46055</v>
       </c>
       <c r="B163" t="n">
@@ -4514,7 +4518,7 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="1" t="n">
+      <c r="A164" s="2" t="n">
         <v>46056</v>
       </c>
       <c r="B164" t="n">
@@ -4539,7 +4543,7 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="1" t="n">
+      <c r="A165" s="2" t="n">
         <v>46057</v>
       </c>
       <c r="B165" t="n">
@@ -4564,7 +4568,7 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="1" t="n">
+      <c r="A166" s="2" t="n">
         <v>46058</v>
       </c>
       <c r="B166" t="n">
@@ -4589,7 +4593,7 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="1" t="n">
+      <c r="A167" s="2" t="n">
         <v>46059</v>
       </c>
       <c r="B167" t="n">
@@ -4614,7 +4618,7 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="1" t="n">
+      <c r="A168" s="2" t="n">
         <v>46060</v>
       </c>
       <c r="B168" t="n">
@@ -4639,7 +4643,7 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="1" t="n">
+      <c r="A169" s="2" t="n">
         <v>46061</v>
       </c>
       <c r="B169" t="n">
@@ -4664,7 +4668,7 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="1" t="n">
+      <c r="A170" s="2" t="n">
         <v>46062</v>
       </c>
       <c r="B170" t="n">
@@ -4689,7 +4693,7 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="1" t="n">
+      <c r="A171" s="2" t="n">
         <v>46063</v>
       </c>
       <c r="B171" t="n">
@@ -4714,7 +4718,7 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="1" t="n">
+      <c r="A172" s="2" t="n">
         <v>46064</v>
       </c>
       <c r="B172" t="n">
@@ -4739,7 +4743,7 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="1" t="n">
+      <c r="A173" s="2" t="n">
         <v>46065</v>
       </c>
       <c r="B173" t="n">
@@ -4764,7 +4768,7 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="1" t="n">
+      <c r="A174" s="2" t="n">
         <v>46066</v>
       </c>
       <c r="B174" t="n">
@@ -4789,7 +4793,7 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="1" t="n">
+      <c r="A175" s="2" t="n">
         <v>46067</v>
       </c>
       <c r="B175" t="n">
@@ -4814,7 +4818,7 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="1" t="n">
+      <c r="A176" s="2" t="n">
         <v>46068</v>
       </c>
       <c r="B176" t="n">
@@ -4839,7 +4843,7 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="1" t="n">
+      <c r="A177" s="2" t="n">
         <v>46069</v>
       </c>
       <c r="B177" t="n">
@@ -4864,7 +4868,7 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="1" t="n">
+      <c r="A178" s="2" t="n">
         <v>46070</v>
       </c>
       <c r="B178" t="n">
@@ -4889,7 +4893,7 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="1" t="n">
+      <c r="A179" s="2" t="n">
         <v>46071</v>
       </c>
       <c r="B179" t="n">
@@ -4914,7 +4918,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="1" t="n">
+      <c r="A180" s="2" t="n">
         <v>46072</v>
       </c>
       <c r="B180" t="n">
@@ -4939,7 +4943,7 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" s="1" t="n">
+      <c r="A181" s="2" t="n">
         <v>46073</v>
       </c>
       <c r="B181" t="n">
@@ -4964,7 +4968,7 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="1" t="n">
+      <c r="A182" s="2" t="n">
         <v>46074</v>
       </c>
       <c r="B182" t="n">
@@ -4989,7 +4993,7 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" s="1" t="n">
+      <c r="A183" s="2" t="n">
         <v>46075</v>
       </c>
       <c r="B183" t="n">
@@ -5014,7 +5018,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="1" t="n">
+      <c r="A184" s="2" t="n">
         <v>46076</v>
       </c>
       <c r="B184" t="n">
@@ -5054,19 +5058,24 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Symbol</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>

</xml_diff>

<commit_message>
feat: backfill real-world portfolio quantities for Feb 24-27 and add QQQ to US Stocks
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G184"/>
+  <dimension ref="A1:G188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5038,6 +5038,114 @@
       </c>
       <c r="G184" t="n">
         <v>2989.41</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2026-02-24</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>571.73</v>
+      </c>
+      <c r="C185" t="n">
+        <v>1483.58</v>
+      </c>
+      <c r="D185" t="n">
+        <v>1696.46</v>
+      </c>
+      <c r="E185" t="n">
+        <v>3751.77</v>
+      </c>
+      <c r="F185" t="n">
+        <v>0.9014</v>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>auto-append</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2026-02-25</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>571.73</v>
+      </c>
+      <c r="C186" t="n">
+        <v>1498.14</v>
+      </c>
+      <c r="D186" t="n">
+        <v>1723.54</v>
+      </c>
+      <c r="E186" t="n">
+        <v>3793.41</v>
+      </c>
+      <c r="F186" t="n">
+        <v>0.9114</v>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>auto-append</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2026-02-26</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>571.73</v>
+      </c>
+      <c r="C187" t="n">
+        <v>1500.24</v>
+      </c>
+      <c r="D187" t="n">
+        <v>1692.01</v>
+      </c>
+      <c r="E187" t="n">
+        <v>3763.98</v>
+      </c>
+      <c r="F187" t="n">
+        <v>0.9043</v>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>auto-append</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>571.73</v>
+      </c>
+      <c r="C188" t="n">
+        <v>1500.24</v>
+      </c>
+      <c r="D188" t="n">
+        <v>1692.01</v>
+      </c>
+      <c r="E188" t="n">
+        <v>3763.98</v>
+      </c>
+      <c r="F188" t="n">
+        <v>0.9043</v>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>auto-append</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -5051,7 +5159,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5108,22 +5216,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.287</v>
+        <v>0.2877491817892204</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>QQQ</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NVIDIA Corp</t>
+          <t>Invesco QQQ Trust</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17.4</v>
+        <v>1.7327</v>
       </c>
     </row>
     <row r="5">
@@ -5138,7 +5246,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1.2254</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>NVIDIA Corp</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(sync): write last_updated back to assets.xlsx timestamps
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -311,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -656,6 +656,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="168" fontId="24" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -32343,7 +32346,7 @@
         </is>
       </c>
       <c r="B2" s="77" t="n">
-        <v>46075.74546296296</v>
+        <v>46082.44681172186</v>
       </c>
       <c r="C2" s="86" t="inlineStr">
         <is>
@@ -32396,7 +32399,9 @@
           <t>更新时间</t>
         </is>
       </c>
-      <c r="H3" s="99" t="n"/>
+      <c r="H3" s="122" t="n">
+        <v>46082.44681172186</v>
+      </c>
       <c r="I3" s="99" t="n"/>
       <c r="J3" s="99" t="n"/>
       <c r="K3" s="99" t="n"/>
@@ -62387,7 +62392,7 @@
     </row>
     <row r="2">
       <c r="A2" s="121" t="n">
-        <v>46076.63113425926</v>
+        <v>46082.44681172186</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
@@ -62416,7 +62421,7 @@
     </row>
     <row r="3">
       <c r="A3" s="121" t="n">
-        <v>46076.63113425926</v>
+        <v>46082.44681172186</v>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
@@ -62445,7 +62450,7 @@
     </row>
     <row r="4">
       <c r="A4" s="121" t="n">
-        <v>46076.63113425926</v>
+        <v>46082.44681172186</v>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
@@ -62474,7 +62479,7 @@
     </row>
     <row r="5">
       <c r="A5" s="121" t="n">
-        <v>46076.63113425926</v>
+        <v>46082.44681172186</v>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
@@ -62503,7 +62508,7 @@
     </row>
     <row r="6">
       <c r="A6" s="121" t="n">
-        <v>46076.63113425926</v>
+        <v>46082.44681172186</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
@@ -62532,7 +62537,7 @@
     </row>
     <row r="7">
       <c r="A7" s="121" t="n">
-        <v>46076.63113425926</v>
+        <v>46082.44681172186</v>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
feat(ai): integrate GLM-5 for enterprise news analysis and historical simulation
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -32751,7 +32751,7 @@
         </is>
       </c>
       <c r="B2" s="77" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.47703024338</v>
       </c>
       <c r="C2" s="86" t="inlineStr">
         <is>
@@ -32805,7 +32805,7 @@
         </is>
       </c>
       <c r="H3" s="122" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.47703024338</v>
       </c>
       <c r="I3" s="99" t="n"/>
       <c r="J3" s="99" t="n"/>
@@ -63199,7 +63199,7 @@
     </row>
     <row r="2">
       <c r="A2" s="121" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.47703024338</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
@@ -63228,7 +63228,7 @@
     </row>
     <row r="3">
       <c r="A3" s="121" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.47703024338</v>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
@@ -63257,7 +63257,7 @@
     </row>
     <row r="4">
       <c r="A4" s="121" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.47703024338</v>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
@@ -63286,7 +63286,7 @@
     </row>
     <row r="5">
       <c r="A5" s="121" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.47703024338</v>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
@@ -63315,7 +63315,7 @@
     </row>
     <row r="6">
       <c r="A6" s="121" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.47703024338</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
@@ -63344,7 +63344,7 @@
     </row>
     <row r="7">
       <c r="A7" s="121" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.47703024338</v>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
fix: make enterprise-news branch pass lint and build
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -32751,7 +32751,7 @@
         </is>
       </c>
       <c r="B2" s="77" t="n">
-        <v>46082.47703024338</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="C2" s="86" t="inlineStr">
         <is>
@@ -32805,7 +32805,7 @@
         </is>
       </c>
       <c r="H3" s="122" t="n">
-        <v>46082.47703024338</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="I3" s="99" t="n"/>
       <c r="J3" s="99" t="n"/>
@@ -63199,7 +63199,7 @@
     </row>
     <row r="2">
       <c r="A2" s="121" t="n">
-        <v>46082.47703024338</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
@@ -63228,7 +63228,7 @@
     </row>
     <row r="3">
       <c r="A3" s="121" t="n">
-        <v>46082.47703024338</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
@@ -63257,7 +63257,7 @@
     </row>
     <row r="4">
       <c r="A4" s="121" t="n">
-        <v>46082.47703024338</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
@@ -63286,7 +63286,7 @@
     </row>
     <row r="5">
       <c r="A5" s="121" t="n">
-        <v>46082.47703024338</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
@@ -63315,7 +63315,7 @@
     </row>
     <row r="6">
       <c r="A6" s="121" t="n">
-        <v>46082.47703024338</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
@@ -63344,7 +63344,7 @@
     </row>
     <row r="7">
       <c r="A7" s="121" t="n">
-        <v>46082.47703024338</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Add enterprise news simulation and GLM historical mode (#2)
* feat(ai): integrate GLM-5 for enterprise news analysis and historical simulation

* fix: make enterprise-news branch pass lint and build

* chore: remove cached python artifacts

* test: fix glm integration unit test payload shape
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -32751,7 +32751,7 @@
         </is>
       </c>
       <c r="B2" s="77" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="C2" s="86" t="inlineStr">
         <is>
@@ -32805,7 +32805,7 @@
         </is>
       </c>
       <c r="H3" s="122" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="I3" s="99" t="n"/>
       <c r="J3" s="99" t="n"/>
@@ -63199,7 +63199,7 @@
     </row>
     <row r="2">
       <c r="A2" s="121" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
@@ -63228,7 +63228,7 @@
     </row>
     <row r="3">
       <c r="A3" s="121" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
@@ -63257,7 +63257,7 @@
     </row>
     <row r="4">
       <c r="A4" s="121" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
@@ -63286,7 +63286,7 @@
     </row>
     <row r="5">
       <c r="A5" s="121" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
@@ -63315,7 +63315,7 @@
     </row>
     <row r="6">
       <c r="A6" s="121" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
@@ -63344,7 +63344,7 @@
     </row>
     <row r="7">
       <c r="A7" s="121" t="n">
-        <v>46082.4658343421</v>
+        <v>46082.50493478077</v>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
chore: process local assets.xlsx updates
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -9987,7 +9987,7 @@
         </is>
       </c>
       <c r="B190" s="64" t="n">
-        <v>1.2677</v>
+        <v>1.2689</v>
       </c>
       <c r="C190" s="64" t="n"/>
       <c r="D190" s="64" t="n"/>
@@ -32751,7 +32751,7 @@
         </is>
       </c>
       <c r="B2" s="77" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.2857022881</v>
       </c>
       <c r="C2" s="86" t="inlineStr">
         <is>
@@ -32805,7 +32805,7 @@
         </is>
       </c>
       <c r="H3" s="122" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.2857022881</v>
       </c>
       <c r="I3" s="99" t="n"/>
       <c r="J3" s="99" t="n"/>
@@ -46654,16 +46654,16 @@
         <v>571.73</v>
       </c>
       <c r="C190" s="117" t="n">
-        <v>1505.08</v>
+        <v>1510.08</v>
       </c>
       <c r="D190" s="117" t="n">
         <v>3199.7</v>
       </c>
       <c r="E190" s="117" t="n">
-        <v>5276.5</v>
+        <v>5281.51</v>
       </c>
       <c r="F190" s="91" t="n">
-        <v>1.2677</v>
+        <v>1.2689</v>
       </c>
       <c r="G190" s="123" t="inlineStr">
         <is>
@@ -63199,7 +63199,7 @@
     </row>
     <row r="2">
       <c r="A2" s="121" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.2857022881</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
@@ -63228,7 +63228,7 @@
     </row>
     <row r="3">
       <c r="A3" s="121" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.2857022881</v>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
@@ -63257,7 +63257,7 @@
     </row>
     <row r="4">
       <c r="A4" s="121" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.2857022881</v>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
@@ -63286,7 +63286,7 @@
     </row>
     <row r="5">
       <c r="A5" s="121" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.2857022881</v>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
@@ -63315,7 +63315,7 @@
     </row>
     <row r="6">
       <c r="A6" s="121" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.2857022881</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
@@ -63344,7 +63344,7 @@
     </row>
     <row r="7">
       <c r="A7" s="121" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.2857022881</v>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
@@ -63365,10 +63365,10 @@
         <v>0.28775</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>5230.5</v>
+        <v>5247.89990234375</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>1505.076375</v>
+        <v>1510.083196899414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add Telegram broadcaster, upgrade AI prompt with portfolio weights & news links
Phase 3 Implementation:
- Add src/telegram_bot.py: Delivery Agent with morning/afternoon/evening broadcasts
- Upgrade briefing_agent.py: veteran CIO persona, weight-aware analysis, anti-boilerplate rules
- Add _enrich_holdings(): computes portfolio weight % for each position
- Fix news URLs: extract real Yahoo Finance article links from yfinance
- Add url field to NewsItem schema in advisor_contract.py
- Include clickable news links in Telegram messages

Pipeline changes:
- news_collector.py: extract and propagate article URLs throughout the pipeline
- extract_data.py: map url field to frontend payload
- telegram_bot.py: format and broadcast portfolio insights via Telegram Bot API
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -9987,7 +9987,7 @@
         </is>
       </c>
       <c r="B190" s="64" t="n">
-        <v>1.2677</v>
+        <v>1.2689</v>
       </c>
       <c r="C190" s="64" t="n"/>
       <c r="D190" s="64" t="n"/>
@@ -32751,7 +32751,7 @@
         </is>
       </c>
       <c r="B2" s="77" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.74882633071</v>
       </c>
       <c r="C2" s="86" t="inlineStr">
         <is>
@@ -32805,7 +32805,7 @@
         </is>
       </c>
       <c r="H3" s="122" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.74882633071</v>
       </c>
       <c r="I3" s="99" t="n"/>
       <c r="J3" s="99" t="n"/>
@@ -46654,16 +46654,16 @@
         <v>571.73</v>
       </c>
       <c r="C190" s="117" t="n">
-        <v>1505.08</v>
+        <v>1510.08</v>
       </c>
       <c r="D190" s="117" t="n">
         <v>3199.7</v>
       </c>
       <c r="E190" s="117" t="n">
-        <v>5276.5</v>
+        <v>5281.51</v>
       </c>
       <c r="F190" s="91" t="n">
-        <v>1.2677</v>
+        <v>1.2689</v>
       </c>
       <c r="G190" s="123" t="inlineStr">
         <is>
@@ -63199,7 +63199,7 @@
     </row>
     <row r="2">
       <c r="A2" s="121" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.74882633071</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
@@ -63228,7 +63228,7 @@
     </row>
     <row r="3">
       <c r="A3" s="121" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.74882633071</v>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
@@ -63257,7 +63257,7 @@
     </row>
     <row r="4">
       <c r="A4" s="121" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.74882633071</v>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
@@ -63286,7 +63286,7 @@
     </row>
     <row r="5">
       <c r="A5" s="121" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.74882633071</v>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
@@ -63315,7 +63315,7 @@
     </row>
     <row r="6">
       <c r="A6" s="121" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.74882633071</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
@@ -63344,7 +63344,7 @@
     </row>
     <row r="7">
       <c r="A7" s="121" t="n">
-        <v>46082.50493478077</v>
+        <v>46082.74882633071</v>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
@@ -63365,10 +63365,10 @@
         <v>0.28775</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>5230.5</v>
+        <v>5247.89990234375</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>1505.076375</v>
+        <v>1510.083196899414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>